<commit_message>
updated screening regex to work for both 'c' and 'c++'
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_C\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="745" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -140,6 +140,111 @@
     <t>Weakness_ID_1</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>WEAKNESS ID 1 (Kingdom:Type:Subtype)</t>
+  </si>
+  <si>
+    <t>WEAKNESS ID 2 (Kingdom:Type:Subtype)</t>
+  </si>
+  <si>
+    <t>WEAKNESS ID 3 (Kingdom:Type:Subtype)</t>
+  </si>
+  <si>
+    <t>WEAKNESS ID 4 (Kingdom:Type:Subtype)</t>
+  </si>
+  <si>
+    <t>WEAKNESS ID 5 (Kingdom:Type:Subtype)</t>
+  </si>
+  <si>
+    <t>XML Schema</t>
+  </si>
+  <si>
+    <t>Tag or Attribute</t>
+  </si>
+  <si>
+    <t>Vulnerabilities/Vulnerability</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>AnalysisInfo/Unified/Context/FunctionDeclarationSourceLocation/path</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>ClassInfo/Kingdom</t>
+  </si>
+  <si>
+    <t>Weakness_ID_2</t>
+  </si>
+  <si>
+    <t>ClassInfo/Type</t>
+  </si>
+  <si>
+    <t>Weakness_ID_3</t>
+  </si>
+  <si>
+    <t>ClassInfo/Subtype</t>
+  </si>
+  <si>
+    <t>Time and State:Insecure Temporary File</t>
+  </si>
+  <si>
+    <t>Line_Number</t>
+  </si>
+  <si>
+    <t>AnalysisInfo/Unified/Context/FunctionDeclarationSourceLocation/line</t>
+  </si>
+  <si>
+    <t>Finding_Type</t>
+  </si>
+  <si>
+    <t>Function_Name</t>
+  </si>
+  <si>
+    <t>AnalysisInfo/Unified/Context/Function/name</t>
+  </si>
+  <si>
+    <t>Vendor Name:</t>
+  </si>
+  <si>
+    <t>Date of Scan:</t>
+  </si>
+  <si>
+    <t>Scan Conductor:</t>
+  </si>
+  <si>
+    <t>Comments:</t>
+  </si>
+  <si>
+    <t>Tool Version:</t>
+  </si>
+  <si>
+    <t>Rule Pack Version:</t>
+  </si>
+  <si>
+    <t>Rules Implemented:</t>
+  </si>
+  <si>
+    <t>Tool Name:</t>
+  </si>
+  <si>
+    <t>HP Fortify</t>
+  </si>
+  <si>
+    <t>Language:</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Contact (email):</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">sourceanalyzer -verbose -debug -Xmx4096m -64 -b </t>
     </r>
@@ -148,7 +253,7 @@
         <b/>
         <i/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -170,7 +275,7 @@
         <b/>
         <i/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -185,31 +290,132 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> touchless </t>
+      <t xml:space="preserve"> touchless</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
         <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;AUTO:bat_file&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sourceanalyzer -verbose -debug -Xmx4096m -64 -b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;AUTO:build_id&gt;</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;AUTO:bat_file&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">sourceanalyzer -verbose -debug -Xmx4096m -64 -b </t>
+      <t xml:space="preserve"> -logfile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
         <i/>
         <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;AUTO:scan_log_filename&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-scan -f </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;AUTO:fpr_file&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -Dcom.fortify.sca.limiters.MaxIndirectResolutionsForCall=256 -Dcom.fortify.sca.limiters.MaxFunPtrsForCall=136</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sourceanalyzer -verbose -debug -Xmx4096m -64 -b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -231,7 +437,7 @@
         <b/>
         <i/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -260,182 +466,6 @@
       <t>-clean</t>
     </r>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">sourceanalyzer -verbose -debug -Xmx4096m -64 -b </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;AUTO:build_id&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -logfile </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;AUTO:scan_log_filename&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -scan -f </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;AUTO:fpr_file&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -Dcom.fortify.sca.limiters.MaxIndirectResolutionsForCall=256 -Dcom.fortify.sca.limiters.MaxFunPtrsForCall=136</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>WEAKNESS ID 1 (Kingdom:Type:Subtype)</t>
-  </si>
-  <si>
-    <t>WEAKNESS ID 2 (Kingdom:Type:Subtype)</t>
-  </si>
-  <si>
-    <t>WEAKNESS ID 3 (Kingdom:Type:Subtype)</t>
-  </si>
-  <si>
-    <t>WEAKNESS ID 4 (Kingdom:Type:Subtype)</t>
-  </si>
-  <si>
-    <t>WEAKNESS ID 5 (Kingdom:Type:Subtype)</t>
-  </si>
-  <si>
-    <t>XML Schema</t>
-  </si>
-  <si>
-    <t>Tag or Attribute</t>
-  </si>
-  <si>
-    <t>Vulnerabilities/Vulnerability</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>AnalysisInfo/Unified/Context/FunctionDeclarationSourceLocation/path</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>ClassInfo/Kingdom</t>
-  </si>
-  <si>
-    <t>Weakness_ID_2</t>
-  </si>
-  <si>
-    <t>ClassInfo/Type</t>
-  </si>
-  <si>
-    <t>Weakness_ID_3</t>
-  </si>
-  <si>
-    <t>ClassInfo/Subtype</t>
-  </si>
-  <si>
-    <t>Time and State:Insecure Temporary File</t>
-  </si>
-  <si>
-    <t>Line_Number</t>
-  </si>
-  <si>
-    <t>AnalysisInfo/Unified/Context/FunctionDeclarationSourceLocation/line</t>
-  </si>
-  <si>
-    <t>Finding_Type</t>
-  </si>
-  <si>
-    <t>Function_Name</t>
-  </si>
-  <si>
-    <t>AnalysisInfo/Unified/Context/Function/name</t>
-  </si>
-  <si>
-    <t>Vendor Name:</t>
-  </si>
-  <si>
-    <t>Date of Scan:</t>
-  </si>
-  <si>
-    <t>Scan Conductor:</t>
-  </si>
-  <si>
-    <t>Comments:</t>
-  </si>
-  <si>
-    <t>Tool Version:</t>
-  </si>
-  <si>
-    <t>Rule Pack Version:</t>
-  </si>
-  <si>
-    <t>Rules Implemented:</t>
-  </si>
-  <si>
-    <t>Tool Name:</t>
-  </si>
-  <si>
-    <t>HP Fortify</t>
-  </si>
-  <si>
-    <t>Language:</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Contact (email):</t>
-  </si>
 </sst>
 </file>
 
@@ -444,7 +474,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,10 +498,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -920,19 +957,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -1180,7 +1217,7 @@
         <v>377</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1567,21 +1604,21 @@
         <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -1589,32 +1626,32 @@
         <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -1622,32 +1659,32 @@
         <v>36</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1660,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1676,7 +1713,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -1684,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1692,12 +1729,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1710,7 +1747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:B51"/>
     </sheetView>
   </sheetViews>
@@ -1723,65 +1760,65 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2" ht="234.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" s="8"/>
     </row>

</xml_diff>